<commit_message>
Add scripts to identify the right prior distributions and modify environment_sheet
</commit_message>
<xml_diff>
--- a/inst/extdata/input/general/environment_sheet.xlsx
+++ b/inst/extdata/input/general/environment_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzamzo\Documents\R\git\kwb.fcr\inst\extdata\input\general\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32BBA90-0C7A-4F8F-A556-23A698888225}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FBE48F-8F20-4D96-A0F8-FE7D747682BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="560" windowWidth="9320" windowHeight="8360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="75">
   <si>
     <t>k_aslAir</t>
   </si>
@@ -302,9 +302,6 @@
   </si>
   <si>
     <t>Amount if the whole daily KJ is consumed as wheat: KJ 12 000 - 16 000 (developed Country), Wheat KJ: 1200 - 1500 /100 g</t>
-  </si>
-  <si>
-    <t>normal</t>
   </si>
   <si>
     <t>FALSE</t>
@@ -772,7 +769,7 @@
   <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1407,19 +1404,19 @@
         <v>45</v>
       </c>
       <c r="D22" s="7">
-        <v>1050</v>
+        <v>700</v>
       </c>
       <c r="E22" s="7">
-        <v>100</v>
+        <v>1300</v>
       </c>
       <c r="F22" s="7">
         <v>0</v>
       </c>
       <c r="G22" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H22" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>75</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>70</v>

</xml_diff>